<commit_message>
New Respiratory and Patient parameters
</commit_message>
<xml_diff>
--- a/test/validation/PatientValidationData.xlsx
+++ b/test/validation/PatientValidationData.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\BioGears\docs\Validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Programming\Pulse\engine-ingmar\test\validation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE3A68A3-9A58-495B-B620-A3499CA9C4F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="900" windowWidth="16290" windowHeight="8910" tabRatio="724"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patient-Validation" sheetId="33" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="66">
   <si>
     <t>Output</t>
   </si>
@@ -211,12 +212,18 @@
   </si>
   <si>
     <t>3f</t>
+  </si>
+  <si>
+    <t>IdealBodyWeight</t>
+  </si>
+  <si>
+    <t>kg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1230,12 +1237,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A2" sqref="A2"/>
+      <selection pane="topRight" activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,30 +1477,40 @@
       <c r="L12" s="26"/>
     </row>
     <row r="13" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="23"/>
+      <c r="A13" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="14"/>
       <c r="K13" s="20"/>
-      <c r="L13" s="26"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L13" s="26" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
+        <v>47</v>
+      </c>
+      <c r="B14" s="25"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="23"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -1503,7 +1520,7 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
@@ -1517,75 +1534,65 @@
       <c r="K15" s="20"/>
       <c r="L15" s="26"/>
     </row>
-    <row r="16" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>37</v>
-      </c>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="J16" s="14"/>
       <c r="K16" s="20"/>
-      <c r="L16" s="26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L16" s="26"/>
+    </row>
+    <row r="17" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="C17" s="20" t="s">
         <v>59</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="18"/>
+      <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
-      <c r="J17" s="14"/>
+      <c r="J17" s="3"/>
       <c r="K17" s="20"/>
       <c r="L17" s="26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="C18" s="20" t="s">
         <v>59</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="18"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -1595,18 +1602,18 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C19" s="20" t="s">
         <v>59</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>37</v>
@@ -1618,21 +1625,21 @@
       <c r="J19" s="14"/>
       <c r="K19" s="20"/>
       <c r="L19" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C20" s="20" t="s">
         <v>59</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>37</v>
@@ -1644,21 +1651,21 @@
       <c r="J20" s="14"/>
       <c r="K20" s="20"/>
       <c r="L20" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C21" s="20" t="s">
         <v>59</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>37</v>
@@ -1670,21 +1677,21 @@
       <c r="J21" s="14"/>
       <c r="K21" s="20"/>
       <c r="L21" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C22" s="20" t="s">
         <v>59</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>37</v>
@@ -1696,56 +1703,54 @@
       <c r="J22" s="14"/>
       <c r="K22" s="20"/>
       <c r="L22" s="26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>34</v>
+        <v>22</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>4</v>
       </c>
       <c r="C23" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="17" t="s">
-        <v>57</v>
+      <c r="D23" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F23" s="15"/>
+      <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
       <c r="J23" s="14"/>
       <c r="K23" s="20"/>
       <c r="L23" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" s="8" customFormat="1" ht="36.75" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C24" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>58</v>
+      <c r="C24" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F24" s="23"/>
+      <c r="F24" s="15"/>
       <c r="G24" s="3"/>
-      <c r="H24" s="11" t="s">
-        <v>40</v>
-      </c>
+      <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="14"/>
       <c r="K24" s="20"/>
@@ -1753,11 +1758,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" s="8" customFormat="1" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="20" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="19" t="s">
@@ -1769,9 +1774,11 @@
       <c r="E25" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F25" s="18"/>
+      <c r="F25" s="23"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="22"/>
+      <c r="H25" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="I25" s="3"/>
       <c r="J25" s="14"/>
       <c r="K25" s="20"/>
@@ -1779,11 +1786,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="24" t="s">
         <v>34</v>
       </c>
       <c r="C26" s="19" t="s">
@@ -1795,11 +1802,9 @@
       <c r="E26" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="23"/>
+      <c r="F26" s="18"/>
       <c r="G26" s="3"/>
-      <c r="H26" s="3" t="s">
-        <v>41</v>
-      </c>
+      <c r="H26" s="22"/>
       <c r="I26" s="3"/>
       <c r="J26" s="14"/>
       <c r="K26" s="20"/>
@@ -1809,7 +1814,7 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B27" s="25" t="s">
         <v>34</v>
@@ -1835,9 +1840,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="36.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B28" s="25" t="s">
         <v>34</v>
@@ -1853,8 +1858,8 @@
       </c>
       <c r="F28" s="23"/>
       <c r="G28" s="3"/>
-      <c r="H28" s="11" t="s">
-        <v>40</v>
+      <c r="H28" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="I28" s="3"/>
       <c r="J28" s="14"/>
@@ -1863,9 +1868,9 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A29" s="10" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B29" s="25" t="s">
         <v>34</v>
@@ -1882,7 +1887,7 @@
       <c r="F29" s="23"/>
       <c r="G29" s="3"/>
       <c r="H29" s="11" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="I29" s="3"/>
       <c r="J29" s="14"/>
@@ -1891,11 +1896,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="25" t="s">
         <v>34</v>
       </c>
       <c r="C30" s="19" t="s">
@@ -1907,9 +1912,11 @@
       <c r="E30" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F30" s="18"/>
+      <c r="F30" s="23"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="22"/>
+      <c r="H30" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="I30" s="3"/>
       <c r="J30" s="14"/>
       <c r="K30" s="20"/>
@@ -1917,6 +1924,32 @@
         <v>63</v>
       </c>
     </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="18"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="26" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>